<commit_message>
Updated Thread.sleep -> Wait
</commit_message>
<xml_diff>
--- a/ExcelFile/SwagLabLoginData.xlsx
+++ b/ExcelFile/SwagLabLoginData.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E99C4929-128B-465F-8667-BC9F81A087D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="2130" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P5"/>
+  <oleSize ref="A1:J18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -422,20 +423,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="15" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
     <col min="2" max="16384" width="15" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -457,7 +458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -468,7 +469,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -479,7 +480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -490,7 +491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -501,7 +502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -512,7 +513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -530,23 +531,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -560,7 +561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -574,12 +575,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
@@ -590,7 +591,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -601,7 +602,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -612,7 +613,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -626,7 +627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -640,7 +641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -654,7 +655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -668,7 +669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -682,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>